<commit_message>
Finished compare offers page - support 2-3 offers
</commit_message>
<xml_diff>
--- a/docs/Requirement/CalculateOffersValues.xlsx
+++ b/docs/Requirement/CalculateOffersValues.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8115" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Offer values" sheetId="1" r:id="rId1"/>
+    <sheet name="cjo offer table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t>Field</t>
   </si>
@@ -92,9 +93,6 @@
     <t>= (Salary/52) x PTO</t>
   </si>
   <si>
-    <t>= (1.5% x Salary)/4</t>
-  </si>
-  <si>
     <t>Calculate values</t>
   </si>
   <si>
@@ -129,6 +127,60 @@
   </si>
   <si>
     <t>Medicaloffered</t>
+  </si>
+  <si>
+    <t>= (3.5% x Salary)/4</t>
+  </si>
+  <si>
+    <t>Offer table</t>
+  </si>
+  <si>
+    <t>UserID</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>ColID</t>
+  </si>
+  <si>
+    <t>OfferType</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>varchar(80)</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>ReimburseExp</t>
+  </si>
+  <si>
+    <t>decimal(8,2)</t>
+  </si>
+  <si>
+    <t>Relocate</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>Normalworkhours</t>
+  </si>
+  <si>
+    <t>float</t>
+  </si>
+  <si>
+    <t>Null Allowed</t>
   </si>
 </sst>
 </file>
@@ -138,8 +190,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -209,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -217,13 +269,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -548,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,13 +627,13 @@
         <v>16</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G1" s="14" t="s">
         <v>1</v>
@@ -595,14 +647,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>105000</v>
+        <v>100000</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D2" s="3">
-        <f>B2</f>
-        <v>105000</v>
+        <v>110000</v>
       </c>
       <c r="G2" t="s">
         <v>6</v>
@@ -619,7 +670,7 @@
         <v>10000</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="3">
         <f>(B3)/4</f>
@@ -627,11 +678,11 @@
       </c>
       <c r="E3" s="9">
         <f>D3/$D$8</f>
-        <v>1.9243579305750869E-2</v>
+        <v>1.8489940761074408E-2</v>
       </c>
       <c r="F3" s="10">
         <f>E3*D$9</f>
-        <v>2.4999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="G3" t="s">
         <v>6</v>
@@ -645,22 +696,22 @@
         <v>9</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="3">
         <f>0.1 * D2</f>
-        <v>10500</v>
+        <v>11000</v>
       </c>
       <c r="E4" s="9">
         <f>D4/$D$8</f>
-        <v>8.0823033084153659E-2</v>
+        <v>8.1355739348727391E-2</v>
       </c>
       <c r="F4" s="10">
         <f>E4*D$9</f>
-        <v>10.5</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -671,25 +722,25 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="5">
-        <v>0.06</v>
+        <v>0.04</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D5" s="3">
         <f>B5*D2</f>
-        <v>6300</v>
+        <v>4400</v>
       </c>
       <c r="E5" s="9">
         <f>D5/$D$8</f>
-        <v>4.8493819850492191E-2</v>
+        <v>3.254229573949096E-2</v>
       </c>
       <c r="F5" s="10">
         <f>E5*D$9</f>
-        <v>6.2999999999999989</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G5" t="s">
         <v>10</v>
@@ -700,22 +751,22 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="3">
         <f>D2/52*B6</f>
-        <v>4038.4615384615386</v>
+        <v>6346.1538461538457</v>
       </c>
       <c r="E6" s="9">
         <f>D6/$D$8</f>
-        <v>3.1085781955443714E-2</v>
+        <v>4.6936003470419652E-2</v>
       </c>
       <c r="F6" s="10">
         <f>E6*D$9</f>
-        <v>4.0384615384615383</v>
+        <v>6.3461538461538467</v>
       </c>
       <c r="G6" t="s">
         <v>3</v>
@@ -729,22 +780,22 @@
         <v>15</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3">
-        <f>0.015*D2</f>
-        <v>1575</v>
+        <f>0.035*D2/4</f>
+        <v>962.50000000000011</v>
       </c>
       <c r="E7" s="9">
         <f>D7/$D$8</f>
-        <v>1.2123454962623048E-2</v>
+        <v>7.1186271930136482E-3</v>
       </c>
       <c r="F7" s="10">
         <f>E7*D$9</f>
-        <v>1.5749999999999997</v>
+        <v>0.96250000000000024</v>
       </c>
       <c r="G7" t="s">
         <v>4</v>
@@ -755,25 +806,25 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="2"/>
       <c r="D8" s="11">
         <f>SUM(D2:D7)</f>
-        <v>129913.46153846153</v>
+        <v>135208.65384615384</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D9" s="7">
         <f>D8/1000</f>
-        <v>129.91346153846152</v>
+        <v>135.20865384615385</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -781,7 +832,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -801,7 +852,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -818,17 +869,15 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="2">
         <v>10</v>
       </c>
-      <c r="D12" s="7">
-        <v>5</v>
-      </c>
+      <c r="D12" s="7"/>
       <c r="F12" s="10"/>
       <c r="G12" t="s">
         <v>4</v>
@@ -842,12 +891,9 @@
         <v>14</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-      <c r="D13">
         <v>4</v>
       </c>
       <c r="G13" t="s">
@@ -859,13 +905,282 @@
     </row>
     <row r="14" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="13">
         <f>SUM(D9:D13)</f>
-        <v>153.91346153846152</v>
+        <v>150.20865384615385</v>
       </c>
       <c r="E14" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>